<commit_message>
ahc y hunt details
</commit_message>
<xml_diff>
--- a/Práctica 2/Memoria/data/vehiculos.xlsx
+++ b/Práctica 2/Memoria/data/vehiculos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Mi unidad\Universidad\Curso_4_Cuatri_7\CdeDatos\cienciadedatos\Práctica 2\Memoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423FC172-CCC0-4DC0-A81E-1A2DFE9A71CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BADDB18-C64B-40BA-AB37-0479C265CF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68EBF6EB-3C51-4FE6-BE4C-7D6F054DFCB0}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Bicicleta</t>
   </si>
   <si>
-    <t>Camion</t>
-  </si>
-  <si>
     <t>tCarnet</t>
   </si>
   <si>
@@ -68,7 +65,10 @@
     <t>nPasajeros</t>
   </si>
   <si>
-    <t>tVehiculo</t>
+    <t>Camión</t>
+  </si>
+  <si>
+    <t>tVehículo</t>
   </si>
 </sst>
 </file>
@@ -104,9 +104,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,22 +423,22 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -496,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,7 +565,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>